<commit_message>
Update dependencies and refactor account management services; remove unused document handling and reporting tools. Enhance account listing functionality and update protobuf version in requirements.
</commit_message>
<xml_diff>
--- a/migration/outputs/no_changed_email.xlsx
+++ b/migration/outputs/no_changed_email.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F138"/>
+  <dimension ref="A1:F145"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -875,11 +875,7 @@
           <t xml:space="preserve">roberto.young13@gmail.com </t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>Javier Larraguivel</t>
-        </is>
-      </c>
+      <c r="F14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -907,11 +903,7 @@
           <t>malcolm.hill89@gmail.com</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>AGM</t>
-        </is>
-      </c>
+      <c r="F15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -939,11 +931,7 @@
           <t>hc@agmtechnology.com</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>AGM</t>
-        </is>
-      </c>
+      <c r="F16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -999,11 +987,7 @@
           <t>ldmontero@gmail.com</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>AGM</t>
-        </is>
-      </c>
+      <c r="F18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1031,11 +1015,7 @@
           <t xml:space="preserve">reddybolan@gmail.com </t>
         </is>
       </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>AGM</t>
-        </is>
-      </c>
+      <c r="F19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1063,11 +1043,7 @@
           <t>ramoncastro06@gmail.com</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>AGM</t>
-        </is>
-      </c>
+      <c r="F20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1095,11 +1071,7 @@
           <t>stephen.toomer2020@yahoo.com</t>
         </is>
       </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>William Railsback</t>
-        </is>
-      </c>
+      <c r="F21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1127,11 +1099,7 @@
           <t>gfischelg94@gmail.com</t>
         </is>
       </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>AGM</t>
-        </is>
-      </c>
+      <c r="F22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1159,68 +1127,64 @@
           <t>josemaruiz.gonzalez@gmail.com</t>
         </is>
       </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>AGM</t>
-        </is>
-      </c>
+      <c r="F23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Seymour Alvarez Murillo</t>
+          <t>VAMS INC.</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>U14823704</t>
+          <t>U1536192</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>seymourlalvarez@mailfence.com</t>
+          <t>vamsinc332@gmail.com</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>seymourlalvarez@mailfence.com</t>
+          <t>vamsinc332@gmail.com</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>seymouram@gmail.com</t>
+          <t>gsazani@yahoo.com</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Juan Carlos Barboza</t>
+          <t>AGM</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>VAMS INC.</t>
+          <t>Freddy Quesada</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>U1536192</t>
+          <t>U1540636</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>vamsinc332@gmail.com</t>
+          <t>ques4865@gmail.com</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>vamsinc332@gmail.com</t>
+          <t>ques4865@gmail.com</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>gsazani@yahoo.com</t>
+          <t>fqmjvh@yahoo.com</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -1232,108 +1196,100 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Freddy Quesada</t>
+          <t>Inversiones de Centroamerica, S.A.</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>U1540636</t>
+          <t>U15476355</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>ques4865@gmail.com</t>
+          <t>invercasasa@mailfence.com</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>ques4865@gmail.com</t>
+          <t>invercasasa@mailfence.com</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>fqmjvh@yahoo.com</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>AGM</t>
-        </is>
-      </c>
+          <t>tradernac@invercasa.com.ni</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Inversiones de Centroamerica, S.A.</t>
+          <t>Asociacion Solidarista de Empleados de Abbott Medical Limitada</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>U15476355</t>
+          <t>U1594500</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>invercasasa@mailfence.com</t>
+          <t>asocjud874@gmail.com</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>invercasasa@mailfence.com</t>
+          <t>asocjud874@gmail.com</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>tradernac@invercasa.com.ni</t>
+          <t>asocjud874@gmail.com</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>AGM</t>
+          <t>Bullish &amp; Bearish</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Asociacion Solidarista de Empleados de Abbott Medical Limitada</t>
+          <t>Federico Pozuelo Navarro and Federico A Pozuelo Aguayo</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>U1594500</t>
+          <t>U16078834</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>asocjud874@gmail.com</t>
+          <t>pozuelofederico@gmail.com</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>asocjud874@gmail.com</t>
+          <t>pozuelofederico@gmail.com</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>asocjud874@gmail.com</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>Bullish &amp; Bearish</t>
-        </is>
-      </c>
+          <t>pozuelofederico@gmail.com</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Federico Pozuelo Navarro and Federico A Pozuelo Aguayo</t>
+          <t>Federico Pozuelo Navarro and Karina Pozuelo Aguayo</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>U16078834</t>
+          <t>U16497845</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1351,132 +1307,116 @@
           <t>pozuelofederico@gmail.com</t>
         </is>
       </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>AGM</t>
-        </is>
-      </c>
+      <c r="F29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Federico Pozuelo Navarro and Karina Pozuelo Aguayo</t>
+          <t>Ricardo Contreras Reyes</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>U16497845</t>
+          <t>U16517614</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>pozuelofederico@gmail.com</t>
+          <t>rcontreras1767@gmail.com</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>pozuelofederico@gmail.com</t>
+          <t>rcontreras1767@gmail.com</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>pozuelofederico@gmail.com</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>AGM</t>
-        </is>
-      </c>
+          <t>contrerascordero@gmail.com</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Ricardo Contreras Reyes</t>
+          <t>Maria F Obando Barth</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>U16517614</t>
+          <t>U17154679</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>rcontreras1767@gmail.com</t>
+          <t>mariafernandaobando87@gmail.com</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>rcontreras1767@gmail.com</t>
+          <t>mariafernandaobando87@gmail.com</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>contrerascordero@gmail.com</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>AGM</t>
-        </is>
-      </c>
+          <t>mariaobandobarth@gmail.com</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Maria F Obando Barth</t>
+          <t>TAMA DIECIOCHO T Y B SOCIEDAD CIVIL</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>U17154679</t>
+          <t>U17241700</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>mariafernandaobando87@gmail.com</t>
+          <t>tamadieciocho@gmail.com</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>mariafernandaobando87@gmail.com</t>
+          <t>tamadieciocho@gmail.com</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>mariaobandobarth@gmail.com</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>AGM</t>
-        </is>
-      </c>
+          <t>jespinach@gmail.com</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>TAMA DIECIOCHO T Y B SOCIEDAD CIVIL</t>
+          <t>Fomento Financiero S.A.</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>U17241700</t>
+          <t>U1809702</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>tamadieciocho@gmail.com</t>
+          <t>fofisa451@gmail.com</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>tamadieciocho@gmail.com</t>
+          <t>fofisa451@gmail.com</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>jespinach@gmail.com</t>
+          <t>edgarruben@fofisa.com</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -1488,27 +1428,27 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Fomento Financiero S.A.</t>
+          <t>Alex Kramarz</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>U1809702</t>
+          <t>U1868325</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>fofisa451@gmail.com</t>
+          <t>alek27361@gmail.com</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>fofisa451@gmail.com</t>
+          <t>alek27361@gmail.com</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>edgarruben@fofisa.com</t>
+          <t>alexkramarz@gmail.com</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -1520,27 +1460,27 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Alex Kramarz</t>
+          <t>Rafael A Gutierrez De Pineres Rivera and Eduardo Gutierrez De Pineres Rivera</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>U1868325</t>
+          <t>U19034739</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>alek27361@gmail.com</t>
+          <t>rafagutierrez@mailfence.com</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>alek27361@gmail.com</t>
+          <t>rafagutierrez@mailfence.com</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>alexkramarz@gmail.com</t>
+          <t>rafa.gutierrez@icloud.co</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -1552,57 +1492,53 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Rafael A Gutierrez De Pineres Rivera and Eduardo Gutierrez De Pineres Rivera</t>
+          <t>Jose J Villa Lopez</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>U19034739</t>
+          <t>U19782483</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>rafagutierrez@mailfence.com</t>
+          <t>josejvillalopez@mailfence.com</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>rafagutierrez@mailfence.com</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>rafa.gutierrez@icloud.co</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>AGM</t>
-        </is>
-      </c>
+          <t>josejvillalopez@mailfence.com</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr"/>
+      <c r="F36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Jose J Villa Lopez</t>
+          <t>Fernando Estrada</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>U19782483</t>
+          <t>U1993798</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>josejvillalopez@mailfence.com</t>
+          <t>estra5712@gmail.com</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>josejvillalopez@mailfence.com</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr"/>
+          <t>estra5712@gmail.com</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>festrada@grupoimprosa.com</t>
+        </is>
+      </c>
       <c r="F37" t="inlineStr">
         <is>
           <t>AGM</t>
@@ -1612,27 +1548,27 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Fernando Estrada</t>
+          <t>Alberto M Cohen Pinto</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>U1993798</t>
+          <t>U20082544</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>estra5712@gmail.com</t>
+          <t>albertocohen@mailfence.com</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>estra5712@gmail.com</t>
+          <t>albertocohen@mailfence.com</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>festrada@grupoimprosa.com</t>
+          <t>albertofc_88@hotmail.com</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -1644,57 +1580,57 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Alberto M Cohen Pinto</t>
+          <t>Roberto Cruz Sibaja and Gloria Sibaja Cordero</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>U20082544</t>
+          <t>U20167050</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>albertocohen@mailfence.com</t>
+          <t>robertocruz123@mailfence.com</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>albertocohen@mailfence.com</t>
+          <t>robertocruz123@mailfence.com</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>albertofc_88@hotmail.com</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr"/>
+          <t>drcruzsibaja@gmail.com</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>AGM</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Roberto Cruz Sibaja and Gloria Sibaja Cordero</t>
+          <t>Karina Sanchez Corrales and Federico Cedeno Otarola</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>U20167050</t>
+          <t>U20358292</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>robertocruz123@mailfence.com</t>
+          <t>karinasanchez@mailfence.com</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>robertocruz123@mailfence.com</t>
-        </is>
-      </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>drcruzsibaja@gmail.com</t>
-        </is>
-      </c>
+          <t>karinasanchez@mailfence.com</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr"/>
       <c r="F40" t="inlineStr"/>
     </row>
     <row r="41">
@@ -1724,22 +1660,22 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Maria E Fernandez Mora</t>
+          <t>Carlos R Gurdian Navas and Ana L Quesada Rodriguez</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>U20470031</t>
+          <t>U20390316</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>mariaefernandez@mailfence.com</t>
+          <t>cargurdian1356@mailfence.com</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>mariaefernandez@mailfence.com</t>
+          <t>cargurdian1356@mailfence.com</t>
         </is>
       </c>
       <c r="E42" t="inlineStr"/>
@@ -1748,29 +1684,25 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Max Goldberg</t>
+          <t>Maria E Fernandez Mora</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>U2124140</t>
+          <t>U20470031</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>horen7952@yahoo.com</t>
+          <t>mariaefernandez@mailfence.com</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>horen7952@yahoo.com</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>max8221@gmail.com</t>
-        </is>
-      </c>
+          <t>mariaefernandez@mailfence.com</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr"/>
       <c r="F43" t="inlineStr">
         <is>
           <t>AGM</t>
@@ -1780,27 +1712,27 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Juan Carlos Amrhein Schofield</t>
+          <t>Max Goldberg</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>U2320672</t>
+          <t>U2124140</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>amrjc3451@gmail.com</t>
+          <t>horen7952@yahoo.com</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>amrjc3451@gmail.com</t>
+          <t>horen7952@yahoo.com</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>juancarlos.amrhein@gmail.com</t>
+          <t>max8221@gmail.com</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -1812,87 +1744,87 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Marco Monge</t>
+          <t>Juan Carlos Amrhein Schofield</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>U2549120</t>
+          <t>U2320672</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>mm9986579@gmail.com</t>
+          <t>amrjc3451@gmail.com</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>mm9986579@gmail.com</t>
-        </is>
-      </c>
-      <c r="E45" t="inlineStr"/>
+          <t>amrjc3451@gmail.com</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>juancarlos.amrhein@gmail.com</t>
+        </is>
+      </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Juan Carlos Barboza</t>
+          <t>AGM</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Natalia Chain</t>
+          <t>Marco Monge</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>U2587699</t>
+          <t>U2549120</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>natic7295@gmail.com</t>
+          <t>mm9986579@gmail.com</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>natic7295@gmail.com</t>
-        </is>
-      </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>nchapiz@gmail.com</t>
-        </is>
-      </c>
+          <t>mm9986579@gmail.com</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr"/>
       <c r="F46" t="inlineStr">
         <is>
-          <t>AGM</t>
+          <t>Juan Carlos Barboza</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Juan Carlos Amrhein Schofield</t>
+          <t>Natalia Chain</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>U2621768</t>
+          <t>U2587699</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>amrjc3451@gmail.com</t>
+          <t>natic7295@gmail.com</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>amrjc3451@gmail.com</t>
+          <t>natic7295@gmail.com</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>juancarlos.amrhein@gmail.com</t>
+          <t>nchapiz@gmail.com</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -1904,59 +1836,59 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>3-101-253000, S.A.</t>
+          <t>Juan Carlos Amrhein Schofield</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>U2621906</t>
+          <t>U2621768</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>3101jema@gmail.com</t>
+          <t>amrjc3451@gmail.com</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>3101jema@gmail.com</t>
+          <t>amrjc3451@gmail.com</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>mjenkins@rapiboxcr.com</t>
+          <t>juancarlos.amrhein@gmail.com</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Juan Carlos Barboza</t>
+          <t>AGM</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Maria d Cob</t>
+          <t>3-101-253000, S.A.</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>U2641772</t>
+          <t>U2621906</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>cobmaria5423@yahoo.com</t>
+          <t>3101jema@gmail.com</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>cobmaria5423@yahoo.com</t>
+          <t>3101jema@gmail.com</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>maria.cob@hotmail.com</t>
+          <t>mjenkins@rapiboxcr.com</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -1968,27 +1900,27 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Daniel Berrocal and Francisco J Berrocal</t>
+          <t>Maria d Cob</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>U3191299</t>
+          <t>U2641772</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>berrocald8794@yahoo.com</t>
+          <t>cobmaria5423@yahoo.com</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>berrocald8794@yahoo.com</t>
+          <t>cobmaria5423@yahoo.com</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>jberrocal357@me.com</t>
+          <t>maria.cob@hotmail.com</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -2000,25 +1932,29 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Shirley Sanchez</t>
+          <t>Daniel Berrocal and Francisco J Berrocal</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>U3207587</t>
+          <t>U3191299</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>shirl7521@gmail.com</t>
+          <t>berrocald8794@yahoo.com</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>shirl7521@gmail.com</t>
-        </is>
-      </c>
-      <c r="E51" t="inlineStr"/>
+          <t>berrocald8794@yahoo.com</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>jberrocal357@me.com</t>
+        </is>
+      </c>
       <c r="F51" t="inlineStr">
         <is>
           <t>Juan Carlos Barboza</t>
@@ -2028,29 +1964,25 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Jose R Pacheco</t>
+          <t>Shirley Sanchez</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>U3208864</t>
+          <t>U3207587</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>pach8712@gmail.com</t>
+          <t>shirl7521@gmail.com</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>pach8712@gmail.com</t>
-        </is>
-      </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>jpacheco@tacobell.co.cr</t>
-        </is>
-      </c>
+          <t>shirl7521@gmail.com</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr"/>
       <c r="F52" t="inlineStr">
         <is>
           <t>Juan Carlos Barboza</t>
@@ -2060,27 +1992,27 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Miguel Alfaro</t>
+          <t>Jose R Pacheco</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>U3229733</t>
+          <t>U3208864</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>mial78632@gmail.com</t>
+          <t>pach8712@gmail.com</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>mial78632@gmail.com</t>
+          <t>pach8712@gmail.com</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>alfarocanton1@gmail.com</t>
+          <t>jpacheco@tacobell.co.cr</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -2092,25 +2024,29 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Oscar Alberto Zuniga</t>
+          <t>Miguel Alfaro</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>U3291633</t>
+          <t>U3229733</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>oazg5364@yahoo.com</t>
+          <t>mial78632@gmail.com</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>oazg5364@yahoo.com</t>
-        </is>
-      </c>
-      <c r="E54" t="inlineStr"/>
+          <t>mial78632@gmail.com</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>alfarocanton1@gmail.com</t>
+        </is>
+      </c>
       <c r="F54" t="inlineStr">
         <is>
           <t>Juan Carlos Barboza</t>
@@ -2120,411 +2056,407 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Popular Valores Puesto de Bolsa Sociedad Anonima</t>
+          <t>Oscar Alberto Zuniga</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>U3364295</t>
+          <t>U3291633</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>pvsa7591@mail.com</t>
+          <t>oazg5364@yahoo.com</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>pvsa7591@mail.com</t>
-        </is>
-      </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>gvargas@popularvalores.com</t>
-        </is>
-      </c>
+          <t>oazg5364@yahoo.com</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr"/>
       <c r="F55" t="inlineStr">
         <is>
-          <t>AGM</t>
+          <t>Juan Carlos Barboza</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Shalen Prasad</t>
+          <t>Popular Valores Puesto de Bolsa Sociedad Anonima</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>U3876124</t>
+          <t>U3364295</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>shlnp6849@mail.com</t>
+          <t>pvsa7591@mail.com</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>shlnp6849@mail.com</t>
+          <t>pvsa7591@mail.com</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>shay@cascadacr.com</t>
+          <t>gvargas@popularvalores.com</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>Gabriela Cambronero</t>
+          <t>AGM</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Oliver Perales</t>
+          <t>Shalen Prasad</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>U3906034</t>
+          <t>U3876124</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>olvrp6372@mail.com</t>
+          <t>shlnp6849@mail.com</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>olvrp6372@mail.com</t>
+          <t>shlnp6849@mail.com</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>oliverperales@gmail.com</t>
+          <t>shay@cascadacr.com</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>Pablo Cardona Vaselli</t>
+          <t>Gabriela Cambronero</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Lepa Loc In Sociedad Anonima</t>
+          <t>Oliver Perales</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>U4225328</t>
+          <t>U3906034</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>paulk521@mail.com</t>
+          <t>olvrp6372@mail.com</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>paulk521@mail.com</t>
+          <t>olvrp6372@mail.com</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>paulkleiman1@yahoo.com</t>
+          <t>oliverperales@gmail.com</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>AGM</t>
+          <t>Pablo Cardona Vaselli</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Monica Lopez and Erick A Barboza</t>
+          <t>Lepa Loc In Sociedad Anonima</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>U4234961</t>
+          <t>U4225328</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>mlopez2905@hotmail.com</t>
+          <t>paulk521@mail.com</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>mlopez2905@hotmail.com</t>
+          <t>paulk521@mail.com</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>erick.barboza05@gmail.com</t>
+          <t>paulkleiman1@yahoo.com</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>Julian Barboza Lopez</t>
+          <t>AGM</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Randall Sancho</t>
+          <t>Monica Lopez and Erick A Barboza</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>U4258190</t>
+          <t>U4234961</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>rnds5621@yahoo.com</t>
+          <t>mlopez2905@hotmail.com</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>rnds5621@yahoo.com</t>
+          <t>mlopez2905@hotmail.com</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>rsancho39@gmail.com</t>
+          <t>erick.barboza05@gmail.com</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>AGM</t>
+          <t>Julian Barboza Lopez</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Ana Lustig</t>
+          <t>Randall Sancho</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>U4300315</t>
+          <t>U4258190</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>anlh9185@mail.com</t>
+          <t>rnds5621@yahoo.com</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>anlh9185@mail.com</t>
+          <t>rnds5621@yahoo.com</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>ANALUSTIG@GMAIL.COM</t>
+          <t>rsancho39@gmail.com</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>Lucrecia Gamboa</t>
+          <t>AGM</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Sindy T Pessoa</t>
+          <t>Ana Lustig</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>U4331101</t>
+          <t>U4300315</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>stpsa5782@yahoo.com</t>
+          <t>anlh9185@mail.com</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>stpsa5782@yahoo.com</t>
+          <t>anlh9185@mail.com</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>sindy-p@hotmail.com</t>
+          <t>ANALUSTIG@GMAIL.COM</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>AGM</t>
+          <t>Lucrecia Gamboa</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Monica Quiros jiminez and Emilio J San Gil vargas</t>
+          <t>Sindy T Pessoa</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>U4605398</t>
+          <t>U4331101</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>mqesg5389@mail.com</t>
+          <t>stpsa5782@yahoo.com</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>mqesg5389@mail.com</t>
+          <t>stpsa5782@yahoo.com</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>quirosjmonica@gmail.com</t>
+          <t>sindy-p@hotmail.com</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>James Stanley Esquivel</t>
+          <t>AGM</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Stefan Wille Lochner and Christian Wille</t>
+          <t>Monica Quiros jiminez and Emilio J San Gil vargas</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>U4619498</t>
+          <t>U4605398</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>stchw8232@mail.com</t>
+          <t>mqesg5389@mail.com</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>stchw8232@mail.com</t>
+          <t>mqesg5389@mail.com</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>swille@biosaludcr.com</t>
+          <t>quirosjmonica@gmail.com</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>Silvia Glenewinkel</t>
+          <t>James Stanley Esquivel</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Alberto Ferrero and Maria M Cerdas</t>
+          <t>Stefan Wille Lochner and Christian Wille</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>U4784715</t>
+          <t>U4619498</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>afmmc2495@mail.com</t>
+          <t>stchw8232@mail.com</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>afmmc2495@mail.com</t>
+          <t>stchw8232@mail.com</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>aferreroa@yahoo.com</t>
+          <t>swille@biosaludcr.com</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>James Stanley Esquivel</t>
+          <t>Silvia Glenewinkel</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Ernesto Aguilar</t>
+          <t>Alberto Ferrero and Maria M Cerdas</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>U5353411</t>
+          <t>U4784715</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>ernestoaguilar01@gmail.com</t>
+          <t>afmmc2495@mail.com</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>ernestoaguilar01@gmail.com</t>
+          <t>afmmc2495@mail.com</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>ernestoaguilar01@gmail.com</t>
+          <t>aferreroa@yahoo.com</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>AGM</t>
+          <t>James Stanley Esquivel</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Sigifredo Sanchez and Laura Rodriguez</t>
+          <t>Ernesto Aguilar</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>U5426158</t>
+          <t>U5353411</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>sisach421@gmail.com</t>
+          <t>ernestoaguilar01@gmail.com</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>sisach421@gmail.com</t>
+          <t>ernestoaguilar01@gmail.com</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>sig122@hotmail.com</t>
+          <t>ernestoaguilar01@gmail.com</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -2536,283 +2468,283 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Julian Barzuna</t>
+          <t>Sigifredo Sanchez and Laura Rodriguez</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>U5586182</t>
+          <t>U5426158</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>jbarz9201@protonmail.com</t>
+          <t>sisach421@gmail.com</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>jbarz9201@protonmail.com</t>
+          <t>sisach421@gmail.com</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>JBARZ9201@PROTONMAIL.COM</t>
+          <t>sig122@hotmail.com</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>Osvaldo Mora</t>
+          <t>AGM</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>InterClear Central de Valores S.A.</t>
+          <t>Julian Barzuna</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>U5674522</t>
+          <t>U5586182</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>interc5722@mail.com</t>
+          <t>jbarz9201@protonmail.com</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>interc5722@mail.com</t>
+          <t>jbarz9201@protonmail.com</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>INTERCLEAR@INTERCLEARCR.COM</t>
+          <t>JBARZ9201@PROTONMAIL.COM</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>AGM</t>
+          <t>Osvaldo Mora</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Rawson Overseas Limited</t>
+          <t>InterClear Central de Valores S.A.</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>U5732371</t>
+          <t>U5674522</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>cvcar2395@mail.com</t>
+          <t>interc5722@mail.com</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>cvcar2395@mail.com</t>
+          <t>interc5722@mail.com</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>carlosvillaloboscarvajal@gmail.com</t>
+          <t>INTERCLEAR@INTERCLEARCR.COM</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>Osvaldo Mora</t>
+          <t>AGM</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Adriana M Cisneros</t>
+          <t>Rawson Overseas Limited</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>U5767909</t>
+          <t>U5732371</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>adcis5634@yahoo.com</t>
+          <t>cvcar2395@mail.com</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>adcis5634@yahoo.com</t>
+          <t>cvcar2395@mail.com</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>adriana.cisneros@gmail.com</t>
+          <t>carlosvillaloboscarvajal@gmail.com</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>Javier Larraguivel</t>
+          <t>Osvaldo Mora</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Sigifredo Sanchez and Laura Rodriguez</t>
+          <t>Adriana M Cisneros</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>U5823735</t>
+          <t>U5767909</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>sisach421@gmail.com</t>
+          <t>adcis5634@yahoo.com</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>sisach421@gmail.com</t>
+          <t>adcis5634@yahoo.com</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>sig122@hotmail.com</t>
+          <t>adriana.cisneros@gmail.com</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>AGM</t>
+          <t>Javier Larraguivel</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Victor M Solano and Paty M Castillo</t>
+          <t>Sigifredo Sanchez and Laura Rodriguez</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>U5865195</t>
+          <t>U5823735</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>vicso5829@mail.com</t>
+          <t>sisach421@gmail.com</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>vicso5829@mail.com</t>
+          <t>sisach421@gmail.com</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>vsolno@yahoo.com</t>
+          <t>sig122@hotmail.com</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>Javier Larraguivel</t>
+          <t>AGM</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Mauricio J Ventura</t>
+          <t>Victor M Solano and Paty M Castillo</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>U5985893</t>
+          <t>U5865195</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>maven9620@protonmail.com</t>
+          <t>vicso5829@mail.com</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>maven9620@protonmail.com</t>
+          <t>vicso5829@mail.com</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>ventura.mauricio@outlook.com</t>
+          <t>vsolno@yahoo.com</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>Lucrecia Gamboa</t>
+          <t>Javier Larraguivel</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Maritza E Hernandez</t>
+          <t>Mauricio J Ventura</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>U6009160</t>
+          <t>U5985893</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>maher6107@yahoo.com</t>
+          <t>maven9620@protonmail.com</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>maher6107@yahoo.com</t>
+          <t>maven9620@protonmail.com</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>transmary22@gmail.com</t>
+          <t>ventura.mauricio@outlook.com</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>Javier Larraguivel</t>
+          <t>Lucrecia Gamboa</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Mayra Abarca Sagot</t>
+          <t>Maritza E Hernandez</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>U6170355</t>
+          <t>U6009160</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>mabar2819@protonmail.com</t>
+          <t>maher6107@yahoo.com</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>mabar2819@protonmail.com</t>
+          <t>maher6107@yahoo.com</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>mayraaba@gmail.com</t>
+          <t>transmary22@gmail.com</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -2824,59 +2756,59 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Alberto J Cubero</t>
+          <t>Mayra Abarca Sagot</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>U6343244</t>
+          <t>U6170355</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>albcu3569@protonmail.com</t>
+          <t>mabar2819@protonmail.com</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>albcu3569@protonmail.com</t>
+          <t>mabar2819@protonmail.com</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>acubero@ice.co.cr</t>
+          <t>mayraaba@gmail.com</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>AGM</t>
+          <t>Javier Larraguivel</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Jose F Vargas</t>
+          <t>Alberto J Cubero</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>U6343516</t>
+          <t>U6343244</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>jfvar9924@protonmail.com</t>
+          <t>albcu3569@protonmail.com</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>jfvar9924@protonmail.com</t>
+          <t>albcu3569@protonmail.com</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>fa.vargas.mu@gmail.com</t>
+          <t>acubero@ice.co.cr</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -2888,27 +2820,27 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Sebastian A Solano</t>
+          <t>Jose F Vargas</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>U6586421</t>
+          <t>U6343516</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>sebso2477@protonmail.com</t>
+          <t>jfvar9924@protonmail.com</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>sebso2477@protonmail.com</t>
+          <t>jfvar9924@protonmail.com</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>sebastian.sm0999@gmail.com</t>
+          <t>fa.vargas.mu@gmail.com</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -2920,128 +2852,128 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Vivian R Troper and Gabriel Filloy</t>
+          <t>Sebastian A Solano</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>U6616743</t>
+          <t>U6586421</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>vivyga1992@mail.com</t>
+          <t>sebso2477@protonmail.com</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>vivyga1992@mail.com</t>
+          <t>sebso2477@protonmail.com</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>vtroper@gmail.com</t>
+          <t>sebastian.sm0999@gmail.com</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>Ernesto Aguilar</t>
+          <t>AGM</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Adriana P Guerrero</t>
+          <t>Vivian R Troper and Gabriel Filloy</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>U7257457</t>
+          <t>U6616743</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>adpag0183@protonmail.com</t>
+          <t>vivyga1992@mail.com</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>adpag0183@protonmail.com</t>
+          <t>vivyga1992@mail.com</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>adrianaguererrob@gmail.com</t>
+          <t>vtroper@gmail.com</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>AGM</t>
+          <t>Ernesto Aguilar</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Marianella Ramirez</t>
+          <t>Adriana P Guerrero</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>U7274535</t>
+          <t>U7257457</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>marabi1574@protonmail.com</t>
+          <t>adpag0183@protonmail.com</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>marabi1574@protonmail.com</t>
+          <t>adpag0183@protonmail.com</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>fitmamacostarica@gmail.com</t>
+          <t>adrianaguererrob@gmail.com</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>Adrian Alvarado</t>
+          <t>AGM</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Luis D Marin</t>
+          <t>Marianella Ramirez</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>U8431143</t>
+          <t>U7274535</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>ldmari6802@protonmail.com</t>
+          <t>marabi1574@protonmail.com</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>ldmari6802@protonmail.com</t>
+          <t>marabi1574@protonmail.com</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>msluisdiego05@gmail.com</t>
+          <t>fitmamacostarica@gmail.com</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>AGM</t>
+          <t>Adrian Alvarado</t>
         </is>
       </c>
     </row>
@@ -3263,11 +3195,7 @@
           <t>javi.cordero1604@gmail.com</t>
         </is>
       </c>
-      <c r="F90" t="inlineStr">
-        <is>
-          <t>AGM</t>
-        </is>
-      </c>
+      <c r="F90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -3355,11 +3283,7 @@
           <t>gustavo.jop@jopco.net</t>
         </is>
       </c>
-      <c r="F93" t="inlineStr">
-        <is>
-          <t>Ana Laura Contreras</t>
-        </is>
-      </c>
+      <c r="F93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -3387,11 +3311,7 @@
           <t>kshannoncrrv@gmail.com</t>
         </is>
       </c>
-      <c r="F94" t="inlineStr">
-        <is>
-          <t>James Stanley Esquivel</t>
-        </is>
-      </c>
+      <c r="F94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -3415,11 +3335,7 @@
         </is>
       </c>
       <c r="E95" t="inlineStr"/>
-      <c r="F95" t="inlineStr">
-        <is>
-          <t>Javier Larraguivel</t>
-        </is>
-      </c>
+      <c r="F95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -3447,11 +3363,7 @@
           <t xml:space="preserve">helgaocampo@gmail.com </t>
         </is>
       </c>
-      <c r="F96" t="inlineStr">
-        <is>
-          <t>AGM</t>
-        </is>
-      </c>
+      <c r="F96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -3479,11 +3391,7 @@
           <t>stephen.toomer2020@yahoo.com</t>
         </is>
       </c>
-      <c r="F97" t="inlineStr">
-        <is>
-          <t>William Railsback</t>
-        </is>
-      </c>
+      <c r="F97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -3511,11 +3419,7 @@
           <t>adiaz@bolsarc.com</t>
         </is>
       </c>
-      <c r="F98" t="inlineStr">
-        <is>
-          <t>AGM</t>
-        </is>
-      </c>
+      <c r="F98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -3543,11 +3447,7 @@
           <t>vasquezrene6@gmail.com</t>
         </is>
       </c>
-      <c r="F99" t="inlineStr">
-        <is>
-          <t>Javier Larraguivel</t>
-        </is>
-      </c>
+      <c r="F99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -3575,11 +3475,7 @@
           <t>hola@anacontrerascr.com</t>
         </is>
       </c>
-      <c r="F100" t="inlineStr">
-        <is>
-          <t>AGM</t>
-        </is>
-      </c>
+      <c r="F100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -3607,11 +3503,7 @@
           <t>pilisaenz7@gmail.com</t>
         </is>
       </c>
-      <c r="F101" t="inlineStr">
-        <is>
-          <t>Javier Larraguivel</t>
-        </is>
-      </c>
+      <c r="F101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -3639,11 +3531,7 @@
           <t>dianacsierra@gmail.com</t>
         </is>
       </c>
-      <c r="F102" t="inlineStr">
-        <is>
-          <t>William Railsback</t>
-        </is>
-      </c>
+      <c r="F102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -3671,11 +3559,7 @@
           <t>adrianfloresgolfin@gmail.com</t>
         </is>
       </c>
-      <c r="F103" t="inlineStr">
-        <is>
-          <t>Adrian Alvarado</t>
-        </is>
-      </c>
+      <c r="F103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -3703,11 +3587,7 @@
           <t>anamariaramirezbiolley@gmail.com</t>
         </is>
       </c>
-      <c r="F104" t="inlineStr">
-        <is>
-          <t>Adrian Alvarado</t>
-        </is>
-      </c>
+      <c r="F104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -3735,11 +3615,7 @@
           <t>ANDREMAINGOT99@GMAIL.COM</t>
         </is>
       </c>
-      <c r="F105" t="inlineStr">
-        <is>
-          <t>AGM</t>
-        </is>
-      </c>
+      <c r="F105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -3767,11 +3643,7 @@
           <t>giovanna.vietor@aeromar.co.cr</t>
         </is>
       </c>
-      <c r="F106" t="inlineStr">
-        <is>
-          <t>Juan Carlos Herrera</t>
-        </is>
-      </c>
+      <c r="F106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -3799,905 +3671,853 @@
           <t>rabrealey@hotmail.com</t>
         </is>
       </c>
-      <c r="F107" t="inlineStr">
-        <is>
-          <t>Javier Larraguivel</t>
-        </is>
-      </c>
+      <c r="F107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Jose M Dejuk Jaikel and Jose A Dejuk Johnson</t>
+          <t>ASOCIACION SOLIDARISTA DE EMPLEADOS DE TICOFRUT S.A. Y AFINES</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>U19188462</t>
+          <t>U18879846</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>josemigueldejuk@mailfence.com</t>
+          <t>ticofrut077@gmail.com</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>josemigueldejuk@mailfence.com</t>
-        </is>
-      </c>
-      <c r="E108" t="inlineStr">
-        <is>
-          <t>jmdejuk@hotmail.com</t>
-        </is>
-      </c>
-      <c r="F108" t="inlineStr"/>
+          <t>ticofrut077@gmail.com</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr"/>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>AGM</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>InterClear Central de Valores Sociedad Anonima</t>
+          <t>Jose M Dejuk Jaikel and Jose A Dejuk Johnson</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>U19548292</t>
+          <t>U19188462</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>interclear5@gmail.com</t>
+          <t>josemigueldejuk@mailfence.com</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>interclear5@gmail.com</t>
+          <t>josemigueldejuk@mailfence.com</t>
         </is>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>adiaz@bolsarc.com</t>
+          <t>jmdejuk@hotmail.com</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>AGM</t>
+          <t>Javier Larraguivel</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Monique Azuola Castro</t>
+          <t>InterClear Central de Valores Sociedad Anonima</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>U19609758</t>
+          <t>U19548292</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>moniqueazuola@gmail.com</t>
+          <t>interclear5@gmail.com</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>moniqueazuola@gmail.com</t>
+          <t>interclear5@gmail.com</t>
         </is>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>mazuola@hotmail.com</t>
-        </is>
-      </c>
-      <c r="F110" t="inlineStr">
-        <is>
-          <t>AGM</t>
-        </is>
-      </c>
+          <t>adiaz@bolsarc.com</t>
+        </is>
+      </c>
+      <c r="F110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Ana Sofia Arguedas Villa</t>
+          <t>Monique Azuola Castro</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>U19973459</t>
+          <t>U19609758</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>anaarg@mailfence.com</t>
+          <t>moniqueazuola@gmail.com</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>anaarg@mailfence.com</t>
+          <t>moniqueazuola@gmail.com</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>sarg.829@gmail.com</t>
-        </is>
-      </c>
-      <c r="F111" t="inlineStr">
-        <is>
-          <t>Ana Laura Contreras</t>
-        </is>
-      </c>
+          <t>mazuola@hotmail.com</t>
+        </is>
+      </c>
+      <c r="F111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Manuel Marenco</t>
+          <t>Ana Sofia Arguedas Villa</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>U2365085</t>
+          <t>U19973459</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>marec651@gmail.com</t>
+          <t>anaarg@mailfence.com</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>marec651@gmail.com</t>
+          <t>anaarg@mailfence.com</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>mmarenco@estrategica.fi.cr</t>
+          <t>sarg.829@gmail.com</t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
         <is>
-          <t>AGM</t>
+          <t>Ana Laura Contreras</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Rolbeed del Oeste Sociedad de Responsabilidad Limitada</t>
+          <t>Antonio Goicoechea Bonilla and Alejandro Goicoechea Garcia</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>U2408781</t>
+          <t>U20392242</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>rolb9761@gmail.com</t>
+          <t>goicoecheaantonio61@gmail.com</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>rolb9761@gmail.com</t>
-        </is>
-      </c>
-      <c r="E113" t="inlineStr">
-        <is>
-          <t>rbeeche@interra.co.cr</t>
-        </is>
-      </c>
-      <c r="F113" t="inlineStr">
-        <is>
-          <t>Osvaldo Mora</t>
-        </is>
-      </c>
+          <t>goicoecheaantonio61@gmail.com</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr"/>
+      <c r="F113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Wendy Delius</t>
+          <t>GBI GEOINTELIGENCIA DE NEGOCIOS LIMITADA</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>U2485633</t>
+          <t>U20430156</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>wede8652@gmail.com</t>
+          <t>tomasfernandez@mailfence.com</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>wede8652@gmail.com</t>
-        </is>
-      </c>
-      <c r="E114" t="inlineStr">
-        <is>
-          <t>wdelius19@gmail.com</t>
-        </is>
-      </c>
+          <t>tomasfernandez@mailfence.com</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr"/>
       <c r="F114" t="inlineStr">
         <is>
-          <t>Sandra Asis</t>
+          <t>AGM</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Gian C Mazzali</t>
+          <t>3-102-899563 SOCIEDAD DE RESPONSABILIDAD LIMITADA</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>U2499172</t>
+          <t>U20566763</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>giancarlom038@gmail.com</t>
+          <t>3102899563@mailfence.com</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>giancarlom038@gmail.com</t>
-        </is>
-      </c>
-      <c r="E115" t="inlineStr">
-        <is>
-          <t>gcmazzali@gmail.com</t>
-        </is>
-      </c>
-      <c r="F115" t="inlineStr">
-        <is>
-          <t>Osvaldo Mora</t>
-        </is>
-      </c>
+          <t>3102899563@mailfence.com</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr"/>
+      <c r="F115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>FOMENTO INVERSIONES SOCIEDAD ANOMINA</t>
+          <t>Nicole Joseph Kada and Allan Barboza Retana</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>U2509791</t>
+          <t>U20580183</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>foinv89224@gmail.com</t>
+          <t>nicolejoseph@mailfence.com</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>foinv89224@gmail.com</t>
-        </is>
-      </c>
-      <c r="E116" t="inlineStr">
-        <is>
-          <t>rgonzalez1606@gmail.com</t>
-        </is>
-      </c>
-      <c r="F116" t="inlineStr">
-        <is>
-          <t>Gabriela Cambronero</t>
-        </is>
-      </c>
+          <t>nicolejoseph@mailfence.com</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr"/>
+      <c r="F116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Arstein Inversiones Sociedad Anonima</t>
+          <t>Nino Castro Carboni and Matias Castro Volio</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>U2677467</t>
+          <t>U20586040</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>steinarst67529@yahoo.com</t>
+          <t>ninocastro906@gmail.com</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>steinarst67529@yahoo.com</t>
-        </is>
-      </c>
-      <c r="E117" t="inlineStr">
-        <is>
-          <t>juancarlos.amrhein@gmail.com</t>
-        </is>
-      </c>
-      <c r="F117" t="inlineStr">
-        <is>
-          <t>Osvaldo Mora</t>
-        </is>
-      </c>
+          <t>ninocastro906@gmail.com</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr"/>
+      <c r="F117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>LOGICOM INVESTMENTS S.A.</t>
+          <t>Lily Wong Chang and Susana Wong Chang</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>U2715494</t>
+          <t>U20661731</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>huik761236@gmail.com</t>
+          <t>lwong747@yahoo.com</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>huik761236@gmail.com</t>
-        </is>
-      </c>
-      <c r="E118" t="inlineStr">
-        <is>
-          <t>eduardodipalma@logisticacomercial.com</t>
-        </is>
-      </c>
-      <c r="F118" t="inlineStr">
-        <is>
-          <t>Osvaldo Mora</t>
-        </is>
-      </c>
+          <t>lwong747@yahoo.com</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr"/>
+      <c r="F118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>Fiorella Di Palma</t>
+          <t>Manuel Marenco</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>U2826432</t>
+          <t>U2365085</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>palmafiorella@yahoo.com</t>
+          <t>marec651@gmail.com</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>palmafiorella@yahoo.com</t>
+          <t>marec651@gmail.com</t>
         </is>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>dipalmafiorella@gmail.com</t>
+          <t>mmarenco@estrategica.fi.cr</t>
         </is>
       </c>
       <c r="F119" t="inlineStr">
         <is>
-          <t>Marielena Cruz</t>
+          <t>AGM</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Ana C Munoz</t>
+          <t>Rolbeed del Oeste Sociedad de Responsabilidad Limitada</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>U2885803</t>
+          <t>U2408781</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>anac48621@yahoo.com</t>
+          <t>rolb9761@gmail.com</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>anac48621@yahoo.com</t>
+          <t>rolb9761@gmail.com</t>
         </is>
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>acmuvi@gmail.com</t>
+          <t>rbeeche@interra.co.cr</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
         <is>
-          <t>Pablo Fernández</t>
+          <t>Osvaldo Mora</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>CORPORACION TIERRARENOSA Sociedad Anonima</t>
+          <t>Wendy Delius</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>U2896919</t>
+          <t>U2485633</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>rotw2382@gmail.com</t>
+          <t>wede8652@gmail.com</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>rotw2382@gmail.com</t>
+          <t>wede8652@gmail.com</t>
         </is>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>raspinall60@gmail.com</t>
+          <t>wdelius19@gmail.com</t>
         </is>
       </c>
       <c r="F121" t="inlineStr">
         <is>
-          <t>AGM</t>
+          <t>Sandra Asis</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>Sandra Shaw</t>
+          <t>Gian C Mazzali</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>U3116251</t>
+          <t>U2499172</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>sandsh6732@yahoo.com</t>
+          <t>giancarlom038@gmail.com</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>sandsh6732@yahoo.com</t>
+          <t>giancarlom038@gmail.com</t>
         </is>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>shawhomersandra@gmail.com</t>
+          <t>gcmazzali@gmail.com</t>
         </is>
       </c>
       <c r="F122" t="inlineStr">
         <is>
-          <t>Wijbrand Tuinstra</t>
+          <t>Osvaldo Mora</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>Helmut Dorsam</t>
+          <t>FOMENTO INVERSIONES SOCIEDAD ANOMINA</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>U3207438</t>
+          <t>U2509791</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>hlds8752@gmail.com</t>
+          <t>foinv89224@gmail.com</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>hlds8752@gmail.com</t>
+          <t>foinv89224@gmail.com</t>
         </is>
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>hdorsam@seaboard.co.cr</t>
+          <t>rgonzalez1606@gmail.com</t>
         </is>
       </c>
       <c r="F123" t="inlineStr">
         <is>
-          <t>Marielena Cruz</t>
+          <t>Gabriela Cambronero</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>Juan Carlos Simon</t>
+          <t>Arstein Inversiones Sociedad Anonima</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>U3212071</t>
+          <t>U2677467</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>jsimon729@yahoo.com</t>
+          <t>steinarst67529@yahoo.com</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>jsimon729@yahoo.com</t>
-        </is>
-      </c>
-      <c r="E124" t="inlineStr"/>
+          <t>steinarst67529@yahoo.com</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>juancarlos.amrhein@gmail.com</t>
+        </is>
+      </c>
       <c r="F124" t="inlineStr">
         <is>
-          <t>Javier Pacheco Pacheco</t>
+          <t>Osvaldo Mora</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>Adrian Torrealba</t>
+          <t>LOGICOM INVESTMENTS S.A.</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>U3293996</t>
+          <t>U2715494</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>adtr2354@mail.com</t>
+          <t>huik761236@gmail.com</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>adtr2354@mail.com</t>
+          <t>huik761236@gmail.com</t>
         </is>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>atorrealba@fayca.com</t>
+          <t>eduardodipalma@logisticacomercial.com</t>
         </is>
       </c>
       <c r="F125" t="inlineStr">
         <is>
-          <t>Gabriela Cambronero</t>
+          <t>Osvaldo Mora</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>Sylvia L Varela</t>
+          <t>Fiorella Di Palma</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>U3430091</t>
+          <t>U2826432</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>sylv0285@mail.com</t>
+          <t>palmafiorella@yahoo.com</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>sylv0285@mail.com</t>
+          <t>palmafiorella@yahoo.com</t>
         </is>
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>sylvia.varela@astrazeneza.com</t>
+          <t>dipalmafiorella@gmail.com</t>
         </is>
       </c>
       <c r="F126" t="inlineStr">
         <is>
-          <t>Osvaldo Mora</t>
+          <t>Marielena Cruz</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>Inmobiliaria de Rioja S.A.</t>
+          <t>Ana C Munoz</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>U3539586</t>
+          <t>U2885803</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>mvug2001@mail.com</t>
+          <t>anac48621@yahoo.com</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>mvug2001@mail.com</t>
+          <t>anac48621@yahoo.com</t>
         </is>
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>mvurgelles@urgelles.com</t>
+          <t>acmuvi@gmail.com</t>
         </is>
       </c>
       <c r="F127" t="inlineStr">
         <is>
-          <t>Gabriela Cambronero</t>
+          <t>Pablo Fernández</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>Manrique Robert</t>
+          <t>CORPORACION TIERRARENOSA Sociedad Anonima</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>U3605912</t>
+          <t>U2896919</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>mnrq4820@mail.com</t>
+          <t>rotw2382@gmail.com</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>mnrq4820@mail.com</t>
+          <t>rotw2382@gmail.com</t>
         </is>
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>mrobert@simpapel.net</t>
+          <t>raspinall60@gmail.com</t>
         </is>
       </c>
       <c r="F128" t="inlineStr">
         <is>
-          <t>Pablo Cardona Vaselli</t>
+          <t>AGM</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>Inmobiliara Alfrava Sociedad Anonima</t>
+          <t>Sandra Shaw</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>U4114557</t>
+          <t>U3116251</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>inmal4587@yahoo.com</t>
+          <t>sandsh6732@yahoo.com</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>inmal4587@yahoo.com</t>
+          <t>sandsh6732@yahoo.com</t>
         </is>
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>inmobiliariaalfrava@gmail.com</t>
+          <t>shawhomersandra@gmail.com</t>
         </is>
       </c>
       <c r="F129" t="inlineStr">
         <is>
-          <t>Osvaldo Mora</t>
+          <t>Wijbrand Tuinstra</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>Rodrigo Esquivel and Vilma Rodriguez Saborio</t>
+          <t>Helmut Dorsam</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>U4346345</t>
+          <t>U3207438</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>revr1935@mail.com</t>
+          <t>hlds8752@gmail.com</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>revr1935@mail.com</t>
+          <t>hlds8752@gmail.com</t>
         </is>
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>rodrigoyvilma@gmail.com</t>
+          <t>hdorsam@seaboard.co.cr</t>
         </is>
       </c>
       <c r="F130" t="inlineStr">
         <is>
-          <t>James Stanley Esquivel</t>
+          <t>Marielena Cruz</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>Andres A Blanco</t>
+          <t>Juan Carlos Simon</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>U5162792</t>
+          <t>U3212071</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>andab8639@mail.com</t>
+          <t>jsimon729@yahoo.com</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>andab8639@mail.com</t>
-        </is>
-      </c>
-      <c r="E131" t="inlineStr">
-        <is>
-          <t>andresblancob@me.com</t>
-        </is>
-      </c>
+          <t>jsimon729@yahoo.com</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr"/>
       <c r="F131" t="inlineStr">
         <is>
-          <t>Javier Larraguivel</t>
+          <t>Javier Pacheco Pacheco</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>Victor M Blanco and Ruth Altamirano</t>
+          <t>Adrian Torrealba</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>U5230023</t>
+          <t>U3293996</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>vmbra1038@protonmail.com</t>
+          <t>adtr2354@mail.com</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>vmbra1038@protonmail.com</t>
+          <t>adtr2354@mail.com</t>
         </is>
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>tecnosolar@live.com</t>
+          <t>atorrealba@fayca.com</t>
         </is>
       </c>
       <c r="F132" t="inlineStr">
         <is>
-          <t>Javier Larraguivel</t>
+          <t>Gabriela Cambronero</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>Costa Rica Trust Services Sociedad de Responsabilidad Limitada</t>
+          <t>Sylvia L Varela</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>U7321123</t>
+          <t>U3430091</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>atls7895@gmail.com</t>
+          <t>sylv0285@mail.com</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>atls7895@gmail.com</t>
+          <t>sylv0285@mail.com</t>
         </is>
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t xml:space="preserve">avillalobos@ilacr.com </t>
+          <t>sylvia.varela@astrazeneza.com</t>
         </is>
       </c>
       <c r="F133" t="inlineStr">
         <is>
-          <t>AGM</t>
+          <t>Osvaldo Mora</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>Inversiones Strandhause Limitada</t>
+          <t>Inmobiliaria de Rioja S.A.</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>U7906488</t>
+          <t>U3539586</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>strand629@mail.com</t>
+          <t>mvug2001@mail.com</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>strand629@mail.com</t>
-        </is>
-      </c>
-      <c r="E134" t="inlineStr"/>
+          <t>mvug2001@mail.com</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>mvurgelles@urgelles.com</t>
+        </is>
+      </c>
       <c r="F134" t="inlineStr">
         <is>
-          <t>James Stanley Esquivel</t>
+          <t>Gabriela Cambronero</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>Daniela Araya Gutierrez</t>
+          <t>Manrique Robert</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>U8869483</t>
+          <t>U3605912</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>danar2839@mail.com</t>
+          <t>mnrq4820@mail.com</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>danar2839@mail.com</t>
+          <t>mnrq4820@mail.com</t>
         </is>
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>DANI.ARAYA26@GMAIL.COM</t>
+          <t>mrobert@simpapel.net</t>
         </is>
       </c>
       <c r="F135" t="inlineStr">
         <is>
-          <t>Juan Carlos Herrera</t>
+          <t>Pablo Cardona Vaselli</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>Alfredo J Atmetlla Van Der Laat</t>
+          <t>Inmobiliara Alfrava Sociedad Anonima</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>U9032477</t>
+          <t>U4114557</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
@@ -4712,7 +4532,7 @@
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>INMOBILIARIAALFRAVA@GMAIL.COM</t>
+          <t>inmobiliariaalfrava@gmail.com</t>
         </is>
       </c>
       <c r="F136" t="inlineStr">
@@ -4724,62 +4544,282 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>Laura Granados Cordoba</t>
+          <t>Rodrigo Esquivel and Vilma Rodriguez Saborio</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>U9347752</t>
+          <t>U4346345</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>cordobalaura67@protonmail.com</t>
+          <t>revr1935@mail.com</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>cordobalaura67@protonmail.com</t>
+          <t>revr1935@mail.com</t>
         </is>
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>lgranados@aerojet.co.cr</t>
+          <t>rodrigoyvilma@gmail.com</t>
         </is>
       </c>
       <c r="F137" t="inlineStr">
         <is>
-          <t>Javier Larraguivel</t>
+          <t>James Stanley Esquivel</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
+          <t>Andres A Blanco</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>U5162792</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>andab8639@mail.com</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>andab8639@mail.com</t>
+        </is>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>andresblancob@me.com</t>
+        </is>
+      </c>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>Javier Larraguivel</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>Victor M Blanco and Ruth Altamirano</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>U5230023</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>vmbra1038@protonmail.com</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>vmbra1038@protonmail.com</t>
+        </is>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>tecnosolar@live.com</t>
+        </is>
+      </c>
+      <c r="F139" t="inlineStr">
+        <is>
+          <t>Javier Larraguivel</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>Costa Rica Trust Services Sociedad de Responsabilidad Limitada</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>U7321123</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>atls7895@gmail.com</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>atls7895@gmail.com</t>
+        </is>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t xml:space="preserve">avillalobos@ilacr.com </t>
+        </is>
+      </c>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>AGM</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>Inversiones Strandhause Limitada</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>U7906488</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>strand629@mail.com</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>strand629@mail.com</t>
+        </is>
+      </c>
+      <c r="E141" t="inlineStr"/>
+      <c r="F141" t="inlineStr">
+        <is>
+          <t>James Stanley Esquivel</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>Daniela Araya Gutierrez</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>U8869483</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>danar2839@mail.com</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>danar2839@mail.com</t>
+        </is>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>DANI.ARAYA26@GMAIL.COM</t>
+        </is>
+      </c>
+      <c r="F142" t="inlineStr">
+        <is>
+          <t>Juan Carlos Herrera</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>Alfredo J Atmetlla Van Der Laat</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>U9032477</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>inmal4587@yahoo.com</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>inmal4587@yahoo.com</t>
+        </is>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>INMOBILIARIAALFRAVA@GMAIL.COM</t>
+        </is>
+      </c>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>Osvaldo Mora</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>Laura Granados Cordoba</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>U9347752</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>cordobalaura67@protonmail.com</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>cordobalaura67@protonmail.com</t>
+        </is>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>lgranados@aerojet.co.cr</t>
+        </is>
+      </c>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>Javier Larraguivel</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
           <t>Marta E Navarro Fernandez and Ana L Pozuelo Navarro</t>
         </is>
       </c>
-      <c r="B138" t="inlineStr">
+      <c r="B145" t="inlineStr">
         <is>
           <t>U9858946</t>
         </is>
       </c>
-      <c r="C138" t="inlineStr">
+      <c r="C145" t="inlineStr">
         <is>
           <t>marta.navarro@email.com</t>
         </is>
       </c>
-      <c r="D138" t="inlineStr">
+      <c r="D145" t="inlineStr">
         <is>
           <t>marta.navarro@email.com</t>
         </is>
       </c>
-      <c r="E138" t="inlineStr">
+      <c r="E145" t="inlineStr">
         <is>
           <t>martaenavarro@yahoo.com</t>
         </is>
       </c>
-      <c r="F138" t="inlineStr">
+      <c r="F145" t="inlineStr">
         <is>
           <t>Federico Pozuelo</t>
         </is>

</xml_diff>